<commit_message>
modified 2005 2006 2007
</commit_message>
<xml_diff>
--- a/FCC/2005.xlsx
+++ b/FCC/2005.xlsx
@@ -10,14 +10,14 @@
     <sheet name="2005" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'2005'!$A$1:$M$252</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'2005'!$A$1:$M$248</definedName>
   </definedNames>
   <calcPr calcId="0" iterate="1" iterateCount="1" iterateDelta="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="237">
   <si>
     <t xml:space="preserve">Andorra                             </t>
   </si>
@@ -728,18 +728,6 @@
   </si>
   <si>
     <t xml:space="preserve">     Carriers serving Misc. U.S. points  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total  for  Foreign  Points         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total  for  U.S.  Points            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Total Non-Confidential Included Above</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Total Confidential Included Above</t>
   </si>
 </sst>
 </file>
@@ -804,15 +792,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="5" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="37" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1115,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M257"/>
+  <dimension ref="A1:M253"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="87" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J65536"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="A229" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A249" sqref="A249:XFD252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11299,211 +11284,47 @@
         <v>4086897</v>
       </c>
     </row>
-    <row r="249" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B249" s="2">
-        <v>13106060411</v>
-      </c>
-      <c r="C249" s="2">
-        <v>69881902275</v>
-      </c>
-      <c r="D249" s="3">
-        <v>7390654146</v>
-      </c>
-      <c r="E249" s="3">
-        <v>4091323513</v>
-      </c>
-      <c r="F249" s="3">
-        <v>3299330633</v>
-      </c>
-      <c r="G249" s="2">
-        <v>5761136884</v>
-      </c>
-      <c r="H249" s="2">
-        <v>21735781345</v>
-      </c>
-      <c r="I249" s="3">
-        <v>631613280</v>
-      </c>
-      <c r="J249" s="3">
-        <v>340397436</v>
-      </c>
-      <c r="K249" s="3">
-        <v>17221662</v>
-      </c>
-      <c r="L249" s="3">
-        <v>323175774</v>
-      </c>
-      <c r="M249" s="3">
-        <v>4254119687</v>
-      </c>
-    </row>
-    <row r="250" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A250" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B250" s="2">
-        <v>28415813</v>
-      </c>
-      <c r="C250" s="2">
-        <v>182214281</v>
-      </c>
-      <c r="D250" s="3">
-        <v>9444179</v>
-      </c>
-      <c r="E250" s="3">
-        <v>6954997</v>
-      </c>
-      <c r="F250" s="3">
-        <v>2489182</v>
-      </c>
-      <c r="G250" s="2">
-        <v>20999259</v>
-      </c>
-      <c r="H250" s="2">
-        <v>129190848</v>
-      </c>
-      <c r="I250" s="3">
-        <v>5812983</v>
-      </c>
-      <c r="J250" s="3">
-        <v>65356</v>
-      </c>
-      <c r="K250" s="3">
-        <v>25930</v>
-      </c>
-      <c r="L250" s="3">
-        <v>39426</v>
-      </c>
-      <c r="M250" s="3">
-        <v>8341591</v>
-      </c>
-    </row>
-    <row r="251" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A251" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B251" s="2">
-        <v>7911040335</v>
-      </c>
-      <c r="C251" s="2">
-        <v>46504915133</v>
-      </c>
-      <c r="D251" s="3">
-        <v>4782610986</v>
-      </c>
-      <c r="E251" s="3">
-        <v>2863535594</v>
-      </c>
-      <c r="F251" s="3">
-        <v>1919075392</v>
-      </c>
-      <c r="G251" s="2">
-        <v>3710756230</v>
-      </c>
-      <c r="H251" s="2">
-        <v>13101199231</v>
-      </c>
-      <c r="I251" s="3">
-        <v>364281819</v>
-      </c>
-      <c r="J251" s="3">
-        <v>340350903</v>
-      </c>
-      <c r="K251" s="3">
-        <v>17121637</v>
-      </c>
-      <c r="L251" s="3">
-        <v>323229266</v>
-      </c>
-      <c r="M251" s="3">
-        <v>2606586477</v>
-      </c>
-    </row>
-    <row r="252" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A252" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B252" s="6">
-        <v>5223435889</v>
-      </c>
-      <c r="C252" s="6">
-        <v>23559201423</v>
-      </c>
-      <c r="D252" s="6">
-        <v>2617487339</v>
-      </c>
-      <c r="E252" s="6">
-        <v>1234742916</v>
-      </c>
-      <c r="F252" s="6">
-        <v>1382744423</v>
-      </c>
-      <c r="G252" s="6">
-        <v>2071379913</v>
-      </c>
-      <c r="H252" s="6">
-        <v>8763772962</v>
-      </c>
-      <c r="I252" s="6">
-        <v>273144444</v>
-      </c>
-      <c r="J252" s="6">
-        <v>111889</v>
-      </c>
-      <c r="K252" s="6">
-        <v>125955</v>
-      </c>
-      <c r="L252" s="6">
-        <v>-14066</v>
-      </c>
-      <c r="M252" s="6">
-        <v>1655874801</v>
-      </c>
-    </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B254" s="6"/>
-      <c r="C254" s="6"/>
-      <c r="D254" s="6"/>
-      <c r="E254" s="6"/>
-      <c r="F254" s="6"/>
-      <c r="G254" s="6"/>
-      <c r="H254" s="6"/>
-      <c r="I254" s="6"/>
-      <c r="J254" s="6"/>
-      <c r="K254" s="6"/>
-      <c r="L254" s="6"/>
-      <c r="M254" s="6"/>
-    </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B255" s="6"/>
-      <c r="C255" s="6"/>
-      <c r="D255" s="6"/>
-      <c r="E255" s="6"/>
-      <c r="F255" s="6"/>
-      <c r="G255" s="6"/>
-      <c r="H255" s="6"/>
-      <c r="I255" s="6"/>
-      <c r="J255" s="6"/>
-      <c r="K255" s="6"/>
-      <c r="L255" s="6"/>
-      <c r="M255" s="6"/>
-    </row>
-    <row r="257" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B257" s="6"/>
-      <c r="C257" s="6"/>
-      <c r="D257" s="6"/>
-      <c r="E257" s="6"/>
-      <c r="F257" s="6"/>
-      <c r="G257" s="6"/>
-      <c r="H257" s="6"/>
-      <c r="I257" s="6"/>
-      <c r="J257" s="6"/>
-      <c r="K257" s="6"/>
-      <c r="L257" s="6"/>
-      <c r="M257" s="6"/>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B250" s="5"/>
+      <c r="C250" s="5"/>
+      <c r="D250" s="5"/>
+      <c r="E250" s="5"/>
+      <c r="F250" s="5"/>
+      <c r="G250" s="5"/>
+      <c r="H250" s="5"/>
+      <c r="I250" s="5"/>
+      <c r="J250" s="5"/>
+      <c r="K250" s="5"/>
+      <c r="L250" s="5"/>
+      <c r="M250" s="5"/>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B251" s="5"/>
+      <c r="C251" s="5"/>
+      <c r="D251" s="5"/>
+      <c r="E251" s="5"/>
+      <c r="F251" s="5"/>
+      <c r="G251" s="5"/>
+      <c r="H251" s="5"/>
+      <c r="I251" s="5"/>
+      <c r="J251" s="5"/>
+      <c r="K251" s="5"/>
+      <c r="L251" s="5"/>
+      <c r="M251" s="5"/>
+    </row>
+    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B253" s="5"/>
+      <c r="C253" s="5"/>
+      <c r="D253" s="5"/>
+      <c r="E253" s="5"/>
+      <c r="F253" s="5"/>
+      <c r="G253" s="5"/>
+      <c r="H253" s="5"/>
+      <c r="I253" s="5"/>
+      <c r="J253" s="5"/>
+      <c r="K253" s="5"/>
+      <c r="L253" s="5"/>
+      <c r="M253" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.495" right="0.3" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>